<commit_message>
decorated README.md ; docker-compose formation completed
</commit_message>
<xml_diff>
--- a/menu_app/admin/Menu.xlsx
+++ b/menu_app/admin/Menu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t.m.borovets\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sonic_tim\PycharmProjects\YLabProject\menu_app\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B6658B-58EE-4553-A3ED-54FD56063DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94836E02-B358-40C7-80A0-6DC12EA75C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,206 +30,206 @@
     <t>Меню</t>
   </si>
   <si>
+    <t>Холодные закуски</t>
+  </si>
+  <si>
+    <t>К пиву</t>
+  </si>
+  <si>
+    <t>Сельдь Бисмарк</t>
+  </si>
+  <si>
+    <t>Традиционное немецкое блюдо из маринованной сельди</t>
+  </si>
+  <si>
+    <t>Мясная тарелка</t>
+  </si>
+  <si>
+    <t>Рыбная тарелка</t>
+  </si>
+  <si>
+    <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
+  </si>
+  <si>
+    <t>Рамен</t>
+  </si>
+  <si>
+    <t>Горячий рамен</t>
+  </si>
+  <si>
+    <t>Дайзу рамен</t>
+  </si>
+  <si>
+    <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
+  </si>
+  <si>
+    <t>Унаги рамен</t>
+  </si>
+  <si>
+    <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
+  </si>
+  <si>
+    <t>Чиизу Рамен</t>
+  </si>
+  <si>
+    <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
+  </si>
+  <si>
+    <t>Алкогольное меню</t>
+  </si>
+  <si>
+    <t>Алкогольные напитки</t>
+  </si>
+  <si>
+    <t>Красные вина</t>
+  </si>
+  <si>
+    <t>Для романтичного вечера</t>
+  </si>
+  <si>
+    <t>Шемен де Пап ля Ноблесс</t>
+  </si>
+  <si>
+    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Рипароссо Монтепульчано</t>
+  </si>
+  <si>
+    <t>Вино красное, сухое</t>
+  </si>
+  <si>
+    <t>Кьянти, Серристори</t>
+  </si>
+  <si>
+    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Виски</t>
+  </si>
+  <si>
+    <t>Для интересных бесед</t>
+  </si>
+  <si>
+    <t>Джемисон</t>
+  </si>
+  <si>
+    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
+  </si>
+  <si>
+    <t>Джек Дэниелс</t>
+  </si>
+  <si>
+    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
+  </si>
+  <si>
+    <t>Чивас Ригал</t>
+  </si>
+  <si>
+    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
+  </si>
+  <si>
+    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+  <si>
+    <t>05360824-639e-471c-a44f-127064d32a99</t>
+  </si>
+  <si>
+    <t>076d79c7-93df-4ebe-8344-b50f9b37f9d5</t>
+  </si>
+  <si>
+    <t>2004d80c-44c4-4560-bafe-a0342a68cba3</t>
+  </si>
+  <si>
+    <t>201e9192-7a1b-4759-9621-13a971afc93c</t>
+  </si>
+  <si>
+    <t>182.99</t>
+  </si>
+  <si>
+    <t>215.36</t>
+  </si>
+  <si>
+    <t>265.57</t>
+  </si>
+  <si>
+    <t>166.47</t>
+  </si>
+  <si>
+    <t>168.25</t>
+  </si>
+  <si>
+    <t>132.88</t>
+  </si>
+  <si>
+    <t>2700.79</t>
+  </si>
+  <si>
+    <t>3100.33</t>
+  </si>
+  <si>
+    <t>1850.42</t>
+  </si>
+  <si>
+    <t>420.78</t>
+  </si>
+  <si>
+    <t>440.11</t>
+  </si>
+  <si>
+    <t>520.08</t>
+  </si>
+  <si>
+    <t>456f895d-27bf-47d4-83a4-29ec3b014325</t>
+  </si>
+  <si>
+    <t>e0484c80-d2bf-4e5d-a31b-eb6a720432ae</t>
+  </si>
+  <si>
+    <t>d37805b8-8efc-41e2-a821-4b07df2e41f0</t>
+  </si>
+  <si>
+    <t>ee888aa9-2b79-467e-a3f9-afe0517245c8</t>
+  </si>
+  <si>
+    <t>1c66e1b2-8c22-473e-a57a-f318c69cab7f</t>
+  </si>
+  <si>
+    <t>d62aeb0b-d08c-48eb-a2e8-7267909b8349</t>
+  </si>
+  <si>
+    <t>7678e942-5576-4abe-981a-20552db8dcbf</t>
+  </si>
+  <si>
+    <t>2d5ea5ff-c72b-4e38-99ec-a6d4a83555cc</t>
+  </si>
+  <si>
+    <t>1d5afff1-f501-42d5-84d6-3d030271b261</t>
+  </si>
+  <si>
+    <t>107815fa-8ff6-4a0e-a913-a6eb4f78c006</t>
+  </si>
+  <si>
+    <t>3a32ef2f-84a8-48b1-b510-6eef82c9db47</t>
+  </si>
+  <si>
+    <t>7be7449d-9895-40a3-92de-3c241426eeb1</t>
+  </si>
+  <si>
+    <t>49d4e0dd-0f6b-4a1f-b307-3f7742e8e0ed</t>
+  </si>
+  <si>
+    <t>8d491c2f-d6b8-4292-b0ac-4f3825a7c67b</t>
+  </si>
+  <si>
     <t>Основное меню</t>
-  </si>
-  <si>
-    <t>Холодные закуски</t>
-  </si>
-  <si>
-    <t>К пиву</t>
-  </si>
-  <si>
-    <t>Сельдь Бисмарк</t>
-  </si>
-  <si>
-    <t>Традиционное немецкое блюдо из маринованной сельди</t>
-  </si>
-  <si>
-    <t>Мясная тарелка</t>
-  </si>
-  <si>
-    <t>Рыбная тарелка</t>
-  </si>
-  <si>
-    <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
-  </si>
-  <si>
-    <t>Рамен</t>
-  </si>
-  <si>
-    <t>Горячий рамен</t>
-  </si>
-  <si>
-    <t>Дайзу рамен</t>
-  </si>
-  <si>
-    <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
-  </si>
-  <si>
-    <t>Унаги рамен</t>
-  </si>
-  <si>
-    <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
-  </si>
-  <si>
-    <t>Чиизу Рамен</t>
-  </si>
-  <si>
-    <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
-  </si>
-  <si>
-    <t>Алкогольное меню</t>
-  </si>
-  <si>
-    <t>Алкогольные напитки</t>
-  </si>
-  <si>
-    <t>Красные вина</t>
-  </si>
-  <si>
-    <t>Для романтичного вечера</t>
-  </si>
-  <si>
-    <t>Шемен де Пап ля Ноблесс</t>
-  </si>
-  <si>
-    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Рипароссо Монтепульчано</t>
-  </si>
-  <si>
-    <t>Вино красное, сухое</t>
-  </si>
-  <si>
-    <t>Кьянти, Серристори</t>
-  </si>
-  <si>
-    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Виски</t>
-  </si>
-  <si>
-    <t>Для интересных бесед</t>
-  </si>
-  <si>
-    <t>Джемисон</t>
-  </si>
-  <si>
-    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
-  </si>
-  <si>
-    <t>Джек Дэниелс</t>
-  </si>
-  <si>
-    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
-  </si>
-  <si>
-    <t>Чивас Ригал</t>
-  </si>
-  <si>
-    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
-  </si>
-  <si>
-    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
-  </si>
-  <si>
-    <t>05360824-639e-471c-a44f-127064d32a99</t>
-  </si>
-  <si>
-    <t>076d79c7-93df-4ebe-8344-b50f9b37f9d5</t>
-  </si>
-  <si>
-    <t>2004d80c-44c4-4560-bafe-a0342a68cba3</t>
-  </si>
-  <si>
-    <t>201e9192-7a1b-4759-9621-13a971afc93c</t>
-  </si>
-  <si>
-    <t>182.99</t>
-  </si>
-  <si>
-    <t>215.36</t>
-  </si>
-  <si>
-    <t>265.57</t>
-  </si>
-  <si>
-    <t>166.47</t>
-  </si>
-  <si>
-    <t>168.25</t>
-  </si>
-  <si>
-    <t>132.88</t>
-  </si>
-  <si>
-    <t>2700.79</t>
-  </si>
-  <si>
-    <t>3100.33</t>
-  </si>
-  <si>
-    <t>1850.42</t>
-  </si>
-  <si>
-    <t>420.78</t>
-  </si>
-  <si>
-    <t>440.11</t>
-  </si>
-  <si>
-    <t>520.08</t>
-  </si>
-  <si>
-    <t>456f895d-27bf-47d4-83a4-29ec3b014325</t>
-  </si>
-  <si>
-    <t>e0484c80-d2bf-4e5d-a31b-eb6a720432ae</t>
-  </si>
-  <si>
-    <t>d37805b8-8efc-41e2-a821-4b07df2e41f0</t>
-  </si>
-  <si>
-    <t>ee888aa9-2b79-467e-a3f9-afe0517245c8</t>
-  </si>
-  <si>
-    <t>1c66e1b2-8c22-473e-a57a-f318c69cab7f</t>
-  </si>
-  <si>
-    <t>d62aeb0b-d08c-48eb-a2e8-7267909b8349</t>
-  </si>
-  <si>
-    <t>7678e942-5576-4abe-981a-20552db8dcbf</t>
-  </si>
-  <si>
-    <t>2d5ea5ff-c72b-4e38-99ec-a6d4a83555cc</t>
-  </si>
-  <si>
-    <t>1d5afff1-f501-42d5-84d6-3d030271b261</t>
-  </si>
-  <si>
-    <t>107815fa-8ff6-4a0e-a913-a6eb4f78c006</t>
-  </si>
-  <si>
-    <t>3a32ef2f-84a8-48b1-b510-6eef82c9db47</t>
-  </si>
-  <si>
-    <t>7be7449d-9895-40a3-92de-3c241426eeb1</t>
-  </si>
-  <si>
-    <t>49d4e0dd-0f6b-4a1f-b307-3f7742e8e0ed</t>
-  </si>
-  <si>
-    <t>8d491c2f-d6b8-4292-b0ac-4f3825a7c67b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -241,6 +241,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -521,10 +526,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -537,296 +542,316 @@
     <col min="6" max="6" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1">
+    <row r="4" spans="1:7" ht="16.5" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7"/>
       <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1796,6 +1821,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>